<commit_message>
added new signals abcde
</commit_message>
<xml_diff>
--- a/Code/Data/Information Technology/DEC start/CTSH.xlsx
+++ b/Code/Data/Information Technology/DEC start/CTSH.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangyining/Desktop/Thesis/Code/Data/Information Technology/DEC start/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9323E5-C69E-2C49-9363-88D7CF31D480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B112075-CBD0-9143-BBAE-DE7EEB9B60CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="14940" windowHeight="9220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CTSH-USA" sheetId="2" r:id="rId1"/>
+    <sheet name="CTSH-US" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>